<commit_message>
Added ability to add new todo and login functionality with .
</commit_message>
<xml_diff>
--- a/Change Log.xlsx
+++ b/Change Log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>If the username and password are forgotten, ask Evan.Lepolt@gmail.com</t>
+  </si>
+  <si>
+    <t>Added ability to add new Todo</t>
+  </si>
+  <si>
+    <t>Modal pops up with necessary fillings. More work should be done so that stuff like 'Email ATO' doesn't show up with 'Is Public' is not checked</t>
+  </si>
+  <si>
+    <t>Set up login and cookies</t>
+  </si>
+  <si>
+    <t>Users can now log in and it is saved as a cookie variable</t>
   </si>
 </sst>
 </file>
@@ -423,15 +435,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
@@ -530,6 +542,28 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A10" s="4">
+        <v>41843</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A11" s="4">
+        <v>41844</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>